<commit_message>
Updating Templates to support multi-site
</commit_message>
<xml_diff>
--- a/Input-Spreadsheet-backup.xlsx
+++ b/Input-Spreadsheet-backup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\tyscott\iac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64501BC2-CB88-4163-BF5C-A37E28CC89A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D02D3F7D-E68D-4A33-AF0B-156EDC39F739}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="803" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1971" uniqueCount="766">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1985" uniqueCount="770">
   <si>
     <t>Type</t>
   </si>
@@ -1982,12 +1982,6 @@
   </si>
   <si>
     <t>saphdi</t>
-  </si>
-  <si>
-    <t>Physical Domains</t>
-  </si>
-  <si>
-    <t>VMM Domains</t>
   </si>
   <si>
     <t>access_phys</t>
@@ -4398,9 +4392,6 @@
     <t>Consumed Contract Interface</t>
   </si>
   <si>
-    <t>Provider Default</t>
-  </si>
-  <si>
     <t>Forwarding Control</t>
   </si>
   <si>
@@ -4435,6 +4426,48 @@
   </si>
   <si>
     <t>ND RA Prefix Policy</t>
+  </si>
+  <si>
+    <t>default_prfgrp</t>
+  </si>
+  <si>
+    <t>APIC</t>
+  </si>
+  <si>
+    <t>Route Profile Association</t>
+  </si>
+  <si>
+    <t>First Hop Security Policy Association</t>
+  </si>
+  <si>
+    <t>ND Policy Association</t>
+  </si>
+  <si>
+    <t>nd</t>
+  </si>
+  <si>
+    <t>IGMP Interface Policy (not currenty supported)</t>
+  </si>
+  <si>
+    <t>igmpIfPol</t>
+  </si>
+  <si>
+    <t>Netflow Monitor Policies</t>
+  </si>
+  <si>
+    <t>l3extOut</t>
+  </si>
+  <si>
+    <t>L3 Out for Route Profile</t>
+  </si>
+  <si>
+    <t>Physical_Domains</t>
+  </si>
+  <si>
+    <t>VMM_Domains</t>
+  </si>
+  <si>
+    <t>Provider Default Contract</t>
   </si>
   <si>
     <r>
@@ -4457,29 +4490,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> - Please Refer to the "Documentation" word document in the Project Root Directory for Guidance.</t>
-    </r>
-  </si>
-  <si>
-    <t>default_prfgrp</t>
-  </si>
-  <si>
-    <t>APIC</t>
-  </si>
-  <si>
-    <t>Route Profile Association</t>
-  </si>
-  <si>
-    <t>First Hop Security Policy Association</t>
-  </si>
-  <si>
-    <t>Netflow Monitor Policies Association</t>
-  </si>
-  <si>
-    <t>ND Policy Association</t>
-  </si>
-  <si>
-    <t>nd</t>
+      <t xml:space="preserve"> - Please Refer to the "Network Policies Help" word document in the Project Root Directory for Guidance.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -4950,7 +4962,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -5245,6 +5257,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color theme="4" tint="0.39994506668294322"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FF0070C0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="4" tint="0.39994506668294322"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF0070C0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -5302,7 +5336,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="17" fillId="33" borderId="7" xfId="2" applyNumberFormat="1">
@@ -5541,9 +5575,6 @@
     <xf numFmtId="49" fontId="17" fillId="33" borderId="7" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="4">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="22" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5552,6 +5583,15 @@
     </xf>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="23" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="24" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="46">
@@ -6046,7 +6086,7 @@
     <row r="2" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13"/>
       <c r="B2" s="67" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="C2" s="67"/>
       <c r="D2" s="67"/>
@@ -6239,7 +6279,7 @@
     <row r="15" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="13"/>
       <c r="B15" s="67" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="C15" s="67"/>
       <c r="D15" s="67"/>
@@ -6311,7 +6351,7 @@
     <row r="20" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="13"/>
       <c r="B20" s="67" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C20" s="67"/>
       <c r="D20" s="67"/>
@@ -6408,7 +6448,7 @@
     <row r="26" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="13"/>
       <c r="B26" s="67" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C26" s="67"/>
       <c r="D26" s="67"/>
@@ -6505,7 +6545,7 @@
     <row r="32" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="13"/>
       <c r="B32" s="67" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="C32" s="67"/>
       <c r="D32" s="67"/>
@@ -6608,7 +6648,7 @@
     <row r="38" spans="1:13" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="56"/>
       <c r="B38" s="70" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="C38" s="70"/>
       <c r="D38" s="70"/>
@@ -6707,7 +6747,7 @@
     <row r="41" spans="1:13" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="42" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="68" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="B42" s="68"/>
       <c r="C42" s="68"/>
@@ -6725,7 +6765,7 @@
     <row r="43" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="13"/>
       <c r="B43" s="67" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="C43" s="67"/>
       <c r="D43" s="67"/>
@@ -6926,7 +6966,7 @@
     <row r="56" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="13"/>
       <c r="B56" s="67" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="C56" s="67"/>
       <c r="D56" s="67"/>
@@ -7415,7 +7455,7 @@
     <row r="79" spans="1:26" s="3" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="13"/>
       <c r="B79" s="67" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="C79" s="67"/>
       <c r="D79" s="67"/>
@@ -7644,10 +7684,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6C40B1F-256F-4272-B63C-E002752961EA}">
-  <dimension ref="A1:AF65"/>
+  <dimension ref="A1:AG65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7683,13 +7723,14 @@
     <col min="29" max="29" width="20.140625" style="5" customWidth="1"/>
     <col min="30" max="30" width="21.28515625" style="5" customWidth="1"/>
     <col min="31" max="31" width="21.7109375" style="5" customWidth="1"/>
-    <col min="32" max="32" width="15.85546875" style="5" customWidth="1"/>
-    <col min="33" max="16384" width="9.140625" style="5"/>
+    <col min="32" max="32" width="22.7109375" style="5" customWidth="1"/>
+    <col min="33" max="33" width="18.5703125" style="5" customWidth="1"/>
+    <col min="34" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:33" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="81" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="B1" s="81"/>
       <c r="C1" s="81"/>
@@ -7711,10 +7752,10 @@
       <c r="S1" s="61"/>
       <c r="T1" s="61"/>
     </row>
-    <row r="2" spans="1:32" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:33" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="80" t="s">
-        <v>758</v>
+        <v>769</v>
       </c>
       <c r="C2" s="80"/>
       <c r="D2" s="80"/>
@@ -7735,142 +7776,142 @@
       <c r="S2" s="80"/>
       <c r="T2" s="80"/>
     </row>
-    <row r="3" spans="1:32" ht="48.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:33" ht="48.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="D3" s="59" t="s">
         <v>502</v>
       </c>
       <c r="E3" s="59" t="s">
+        <v>596</v>
+      </c>
+      <c r="F3" s="59" t="s">
+        <v>597</v>
+      </c>
+      <c r="G3" s="59" t="s">
         <v>598</v>
       </c>
-      <c r="F3" s="59" t="s">
+      <c r="H3" s="59" t="s">
+        <v>602</v>
+      </c>
+      <c r="I3" s="59" t="s">
+        <v>705</v>
+      </c>
+      <c r="J3" s="59" t="s">
+        <v>706</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>708</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>710</v>
+      </c>
+      <c r="M3" s="59" t="s">
+        <v>697</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>699</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>707</v>
+      </c>
+      <c r="P3" s="8" t="s">
         <v>599</v>
       </c>
-      <c r="G3" s="59" t="s">
+      <c r="Q3" s="8" t="s">
         <v>600</v>
       </c>
-      <c r="H3" s="59" t="s">
-        <v>604</v>
-      </c>
-      <c r="I3" s="59" t="s">
-        <v>707</v>
-      </c>
-      <c r="J3" s="59" t="s">
-        <v>708</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>710</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>712</v>
-      </c>
-      <c r="M3" s="59" t="s">
-        <v>699</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>701</v>
-      </c>
-      <c r="O3" s="8" t="s">
+      <c r="R3" s="59" t="s">
+        <v>715</v>
+      </c>
+      <c r="S3" s="8" t="s">
         <v>709</v>
       </c>
-      <c r="P3" s="8" t="s">
-        <v>601</v>
-      </c>
-      <c r="Q3" s="8" t="s">
-        <v>602</v>
-      </c>
-      <c r="R3" s="59" t="s">
-        <v>717</v>
-      </c>
-      <c r="S3" s="8" t="s">
-        <v>711</v>
-      </c>
       <c r="T3" s="8"/>
     </row>
-    <row r="4" spans="1:32" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:33" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="C4" s="59" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="D4" s="59" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="E4" s="59" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="F4" s="59" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="G4" s="59" t="s">
+        <v>613</v>
+      </c>
+      <c r="H4" s="59" t="s">
+        <v>620</v>
+      </c>
+      <c r="I4" s="59" t="s">
+        <v>623</v>
+      </c>
+      <c r="J4" s="59" t="s">
+        <v>624</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>653</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>711</v>
+      </c>
+      <c r="M4" s="59" t="s">
+        <v>626</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>625</v>
+      </c>
+      <c r="O4" s="8" t="s">
+        <v>627</v>
+      </c>
+      <c r="P4" s="8" t="s">
+        <v>651</v>
+      </c>
+      <c r="Q4" s="59" t="s">
+        <v>614</v>
+      </c>
+      <c r="R4" s="59" t="s">
         <v>615</v>
       </c>
-      <c r="H4" s="59" t="s">
-        <v>622</v>
-      </c>
-      <c r="I4" s="59" t="s">
-        <v>625</v>
-      </c>
-      <c r="J4" s="59" t="s">
-        <v>626</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>655</v>
-      </c>
-      <c r="L4" s="8" t="s">
-        <v>713</v>
-      </c>
-      <c r="M4" s="59" t="s">
-        <v>628</v>
-      </c>
-      <c r="N4" s="8" t="s">
-        <v>627</v>
-      </c>
-      <c r="O4" s="8" t="s">
-        <v>629</v>
-      </c>
-      <c r="P4" s="8" t="s">
-        <v>653</v>
-      </c>
-      <c r="Q4" s="59" t="s">
-        <v>616</v>
-      </c>
-      <c r="R4" s="59" t="s">
-        <v>617</v>
-      </c>
       <c r="S4" s="8" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="T4" s="8"/>
     </row>
-    <row r="5" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:33" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
         <v>161</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="C5" s="28"/>
       <c r="D5" s="28"/>
       <c r="E5" s="18" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="G5" s="18" t="s">
         <v>21</v>
       </c>
       <c r="H5" s="19" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="I5" s="28" t="s">
         <v>65</v>
@@ -7898,33 +7939,33 @@
         <v>53</v>
       </c>
       <c r="R5" s="18" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="S5" s="28" t="s">
         <v>65</v>
       </c>
       <c r="T5" s="28"/>
     </row>
-    <row r="6" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:33" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="23" t="s">
         <v>161</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="C6" s="29"/>
       <c r="D6" s="29"/>
       <c r="E6" s="22" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="F6" s="23" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="G6" s="22" t="s">
         <v>21</v>
       </c>
       <c r="H6" s="23" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="I6" s="29"/>
       <c r="J6" s="29"/>
@@ -7942,25 +7983,25 @@
         <v>53</v>
       </c>
       <c r="R6" s="22" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="S6" s="29"/>
       <c r="T6" s="29"/>
     </row>
-    <row r="7" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:33" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="19" t="s">
         <v>161</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="C7" s="28"/>
       <c r="D7" s="28"/>
       <c r="E7" s="18" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="G7" s="18" t="s">
         <v>21</v>
@@ -7994,14 +8035,14 @@
         <v>53</v>
       </c>
       <c r="R7" s="18" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="S7" s="28" t="s">
         <v>65</v>
       </c>
       <c r="T7" s="28"/>
     </row>
-    <row r="8" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:33" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="23"/>
       <c r="B8" s="23"/>
       <c r="C8" s="29"/>
@@ -8023,9 +8064,9 @@
       <c r="S8" s="29"/>
       <c r="T8" s="29"/>
     </row>
-    <row r="10" spans="1:32" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:33" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="78" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="B10" s="78"/>
       <c r="C10" s="78"/>
@@ -8058,11 +8099,12 @@
       <c r="AD10" s="60"/>
       <c r="AE10" s="60"/>
       <c r="AF10" s="60"/>
-    </row>
-    <row r="11" spans="1:32" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AG10" s="60"/>
+    </row>
+    <row r="11" spans="1:33" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="11"/>
       <c r="B11" s="80" t="s">
-        <v>758</v>
+        <v>769</v>
       </c>
       <c r="C11" s="80"/>
       <c r="D11" s="80"/>
@@ -8094,69 +8136,71 @@
       <c r="AD11" s="11"/>
       <c r="AE11" s="11"/>
       <c r="AF11" s="11"/>
-    </row>
-    <row r="12" spans="1:32" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="83"/>
-      <c r="B12" s="84"/>
-      <c r="C12" s="85"/>
-      <c r="D12" s="82" t="s">
+      <c r="AG11" s="11"/>
+    </row>
+    <row r="12" spans="1:33" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="82"/>
+      <c r="B12" s="83"/>
+      <c r="C12" s="85" t="s">
+        <v>716</v>
+      </c>
+      <c r="D12" s="86"/>
+      <c r="E12" s="86"/>
+      <c r="F12" s="86"/>
+      <c r="G12" s="86"/>
+      <c r="H12" s="86"/>
+      <c r="I12" s="86"/>
+      <c r="J12" s="86"/>
+      <c r="K12" s="86"/>
+      <c r="L12" s="86"/>
+      <c r="M12" s="86"/>
+      <c r="N12" s="86"/>
+      <c r="O12" s="86"/>
+      <c r="P12" s="86"/>
+      <c r="Q12" s="86"/>
+      <c r="R12" s="86"/>
+      <c r="S12" s="86"/>
+      <c r="T12" s="87"/>
+      <c r="U12" s="82" t="s">
+        <v>717</v>
+      </c>
+      <c r="V12" s="83"/>
+      <c r="W12" s="83"/>
+      <c r="X12" s="83"/>
+      <c r="Y12" s="83"/>
+      <c r="Z12" s="84"/>
+      <c r="AA12" s="82" t="s">
         <v>718</v>
       </c>
-      <c r="E12" s="82"/>
-      <c r="F12" s="82"/>
-      <c r="G12" s="82"/>
-      <c r="H12" s="82"/>
-      <c r="I12" s="82"/>
-      <c r="J12" s="82"/>
-      <c r="K12" s="82"/>
-      <c r="L12" s="82"/>
-      <c r="M12" s="82"/>
-      <c r="N12" s="82"/>
-      <c r="O12" s="82"/>
-      <c r="P12" s="82"/>
-      <c r="Q12" s="82"/>
-      <c r="R12" s="82"/>
-      <c r="S12" s="82"/>
-      <c r="T12" s="82"/>
-      <c r="U12" s="83" t="s">
+      <c r="AB12" s="83"/>
+      <c r="AC12" s="84"/>
+      <c r="AD12" s="82" t="s">
         <v>719</v>
       </c>
-      <c r="V12" s="84"/>
-      <c r="W12" s="84"/>
-      <c r="X12" s="84"/>
-      <c r="Y12" s="85"/>
-      <c r="Z12" s="83" t="s">
-        <v>720</v>
-      </c>
-      <c r="AA12" s="84"/>
-      <c r="AB12" s="85"/>
-      <c r="AC12" s="83" t="s">
-        <v>721</v>
-      </c>
-      <c r="AD12" s="84"/>
-      <c r="AE12" s="84"/>
-      <c r="AF12" s="85"/>
-    </row>
-    <row r="13" spans="1:32" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AE12" s="83"/>
+      <c r="AF12" s="83"/>
+      <c r="AG12" s="84"/>
+    </row>
+    <row r="13" spans="1:33" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="D13" s="57" t="s">
         <v>502</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>492</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="I13" s="8" t="s">
         <v>494</v>
@@ -8171,194 +8215,202 @@
         <v>497</v>
       </c>
       <c r="M13" s="8" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="N13" s="8" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="O13" s="8" t="s">
-        <v>698</v>
+        <v>761</v>
       </c>
       <c r="P13" s="8" t="s">
         <v>493</v>
       </c>
       <c r="Q13" s="8" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="R13" s="8" t="s">
+        <v>697</v>
+      </c>
+      <c r="S13" s="8" t="s">
+        <v>696</v>
+      </c>
+      <c r="T13" s="8" t="s">
+        <v>698</v>
+      </c>
+      <c r="U13" s="8" t="s">
+        <v>584</v>
+      </c>
+      <c r="V13" s="8" t="s">
+        <v>585</v>
+      </c>
+      <c r="W13" s="8" t="s">
+        <v>765</v>
+      </c>
+      <c r="X13" s="8" t="s">
+        <v>757</v>
+      </c>
+      <c r="Y13" s="8" t="s">
+        <v>759</v>
+      </c>
+      <c r="Z13" s="8" t="s">
+        <v>587</v>
+      </c>
+      <c r="AA13" s="8" t="s">
+        <v>702</v>
+      </c>
+      <c r="AB13" s="8" t="s">
+        <v>701</v>
+      </c>
+      <c r="AC13" s="8" t="s">
+        <v>700</v>
+      </c>
+      <c r="AD13" s="8" t="s">
         <v>699</v>
       </c>
-      <c r="S13" s="8" t="s">
-        <v>698</v>
-      </c>
-      <c r="T13" s="8" t="s">
-        <v>700</v>
-      </c>
-      <c r="U13" s="8" t="s">
-        <v>586</v>
-      </c>
-      <c r="V13" s="8" t="s">
-        <v>587</v>
-      </c>
-      <c r="W13" s="8" t="s">
-        <v>761</v>
-      </c>
-      <c r="X13" s="8" t="s">
-        <v>764</v>
-      </c>
-      <c r="Y13" s="8" t="s">
-        <v>589</v>
-      </c>
-      <c r="Z13" s="8" t="s">
-        <v>704</v>
-      </c>
-      <c r="AA13" s="8" t="s">
-        <v>703</v>
-      </c>
-      <c r="AB13" s="8" t="s">
-        <v>702</v>
-      </c>
-      <c r="AC13" s="8" t="s">
-        <v>701</v>
-      </c>
-      <c r="AD13" s="8" t="s">
-        <v>762</v>
-      </c>
       <c r="AE13" s="8" t="s">
+        <v>758</v>
+      </c>
+      <c r="AF13" s="8" t="s">
         <v>763</v>
       </c>
-      <c r="AF13" s="8" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="14" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AG13" s="8" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="C14" s="59" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="D14" s="8" t="s">
+        <v>609</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>644</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>638</v>
+      </c>
+      <c r="G14" s="8" t="s">
         <v>611</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="H14" s="8" t="s">
+        <v>629</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>640</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>641</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>643</v>
+      </c>
+      <c r="L14" s="8" t="s">
+        <v>637</v>
+      </c>
+      <c r="M14" s="8" t="s">
+        <v>636</v>
+      </c>
+      <c r="N14" s="8" t="s">
+        <v>633</v>
+      </c>
+      <c r="O14" s="8" t="s">
+        <v>762</v>
+      </c>
+      <c r="P14" s="8" t="s">
+        <v>628</v>
+      </c>
+      <c r="Q14" s="8" t="s">
+        <v>634</v>
+      </c>
+      <c r="R14" s="8" t="s">
+        <v>626</v>
+      </c>
+      <c r="S14" s="8" t="s">
         <v>646</v>
       </c>
-      <c r="F14" s="8" t="s">
-        <v>640</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>613</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>631</v>
-      </c>
-      <c r="I14" s="8" t="s">
-        <v>642</v>
-      </c>
-      <c r="J14" s="8" t="s">
-        <v>643</v>
-      </c>
-      <c r="K14" s="8" t="s">
-        <v>645</v>
-      </c>
-      <c r="L14" s="8" t="s">
+      <c r="T14" s="8" t="s">
+        <v>647</v>
+      </c>
+      <c r="U14" s="8" t="s">
         <v>639</v>
       </c>
-      <c r="M14" s="8" t="s">
-        <v>638</v>
-      </c>
-      <c r="N14" s="8" t="s">
+      <c r="V14" s="8" t="s">
         <v>635</v>
       </c>
-      <c r="O14" s="8" t="s">
-        <v>648</v>
-      </c>
-      <c r="P14" s="8" t="s">
-        <v>630</v>
-      </c>
-      <c r="Q14" s="8" t="s">
-        <v>636</v>
-      </c>
-      <c r="R14" s="8" t="s">
-        <v>628</v>
-      </c>
-      <c r="S14" s="8" t="s">
-        <v>648</v>
-      </c>
-      <c r="T14" s="8" t="s">
-        <v>649</v>
-      </c>
-      <c r="U14" s="8" t="s">
-        <v>641</v>
-      </c>
-      <c r="V14" s="8" t="s">
-        <v>637</v>
-      </c>
       <c r="W14" s="8" t="s">
-        <v>652</v>
+        <v>764</v>
       </c>
       <c r="X14" s="8" t="s">
         <v>650</v>
       </c>
       <c r="Y14" s="8" t="s">
-        <v>644</v>
+        <v>648</v>
       </c>
       <c r="Z14" s="8" t="s">
-        <v>633</v>
+        <v>642</v>
       </c>
       <c r="AA14" s="8" t="s">
+        <v>631</v>
+      </c>
+      <c r="AB14" s="8" t="s">
+        <v>630</v>
+      </c>
+      <c r="AC14" s="8" t="s">
+        <v>612</v>
+      </c>
+      <c r="AD14" s="8" t="s">
+        <v>625</v>
+      </c>
+      <c r="AE14" s="8" t="s">
+        <v>645</v>
+      </c>
+      <c r="AF14" s="8" t="s">
+        <v>649</v>
+      </c>
+      <c r="AG14" s="8" t="s">
         <v>632</v>
       </c>
-      <c r="AB14" s="8" t="s">
-        <v>614</v>
-      </c>
-      <c r="AC14" s="8" t="s">
-        <v>627</v>
-      </c>
-      <c r="AD14" s="8" t="s">
-        <v>647</v>
-      </c>
-      <c r="AE14" s="8" t="s">
-        <v>651</v>
-      </c>
-      <c r="AF14" s="8" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="15" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:33" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="19" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="C15" s="28"/>
       <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
+      <c r="E15" s="28" t="s">
+        <v>65</v>
+      </c>
       <c r="F15" s="28" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="G15" s="19" t="s">
         <v>21</v>
       </c>
       <c r="H15" s="19" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="I15" s="19" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="J15" s="19" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="K15" s="19" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="L15" s="28" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="M15" s="19" t="s">
         <v>21</v>
@@ -8389,60 +8441,63 @@
       </c>
       <c r="V15" s="28"/>
       <c r="W15" s="28"/>
-      <c r="X15" s="28" t="s">
+      <c r="X15" s="28"/>
+      <c r="Y15" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="Y15" s="28"/>
-      <c r="Z15" s="19" t="s">
-        <v>21</v>
-      </c>
+      <c r="Z15" s="28"/>
       <c r="AA15" s="19" t="s">
         <v>21</v>
       </c>
       <c r="AB15" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="AC15" s="28" t="s">
-        <v>65</v>
+      <c r="AC15" s="19" t="s">
+        <v>21</v>
       </c>
       <c r="AD15" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="AE15" s="28"/>
-      <c r="AF15" s="19" t="s">
+      <c r="AE15" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF15" s="28"/>
+      <c r="AG15" s="19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:33" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="23" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="C16" s="29"/>
       <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
+      <c r="E16" s="29" t="s">
+        <v>65</v>
+      </c>
       <c r="F16" s="29" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="G16" s="23" t="s">
         <v>21</v>
       </c>
       <c r="H16" s="23" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="I16" s="23" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="J16" s="23" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="K16" s="23" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="L16" s="29" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="M16" s="23" t="s">
         <v>21</v>
@@ -8473,60 +8528,63 @@
       </c>
       <c r="V16" s="29"/>
       <c r="W16" s="29"/>
-      <c r="X16" s="29" t="s">
+      <c r="X16" s="29"/>
+      <c r="Y16" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="Y16" s="29"/>
-      <c r="Z16" s="23" t="s">
-        <v>21</v>
-      </c>
+      <c r="Z16" s="29"/>
       <c r="AA16" s="23" t="s">
         <v>21</v>
       </c>
       <c r="AB16" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="AC16" s="29" t="s">
-        <v>65</v>
+      <c r="AC16" s="23" t="s">
+        <v>21</v>
       </c>
       <c r="AD16" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="AE16" s="29"/>
-      <c r="AF16" s="23" t="s">
+      <c r="AE16" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF16" s="29"/>
+      <c r="AG16" s="23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:33" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="19" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="C17" s="28"/>
       <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
+      <c r="E17" s="28" t="s">
+        <v>65</v>
+      </c>
       <c r="F17" s="28" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="G17" s="19" t="s">
         <v>22</v>
       </c>
       <c r="H17" s="19" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="I17" s="19" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="J17" s="19" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="K17" s="19" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="L17" s="28" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="M17" s="19" t="s">
         <v>21</v>
@@ -8557,60 +8615,63 @@
       </c>
       <c r="V17" s="28"/>
       <c r="W17" s="28"/>
-      <c r="X17" s="28" t="s">
+      <c r="X17" s="28"/>
+      <c r="Y17" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="Y17" s="28"/>
-      <c r="Z17" s="19" t="s">
-        <v>21</v>
-      </c>
+      <c r="Z17" s="28"/>
       <c r="AA17" s="19" t="s">
         <v>21</v>
       </c>
       <c r="AB17" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="AC17" s="28" t="s">
-        <v>65</v>
+      <c r="AC17" s="19" t="s">
+        <v>21</v>
       </c>
       <c r="AD17" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="AE17" s="28"/>
-      <c r="AF17" s="19" t="s">
+      <c r="AE17" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF17" s="28"/>
+      <c r="AG17" s="19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:33" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="23" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="C18" s="29"/>
       <c r="D18" s="29"/>
-      <c r="E18" s="29"/>
+      <c r="E18" s="29" t="s">
+        <v>65</v>
+      </c>
       <c r="F18" s="29" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="G18" s="23" t="s">
         <v>21</v>
       </c>
       <c r="H18" s="23" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="I18" s="23" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="J18" s="23" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="K18" s="23" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="L18" s="29" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="M18" s="23" t="s">
         <v>21</v>
@@ -8641,60 +8702,63 @@
       </c>
       <c r="V18" s="29"/>
       <c r="W18" s="29"/>
-      <c r="X18" s="29" t="s">
+      <c r="X18" s="29"/>
+      <c r="Y18" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="Y18" s="29"/>
-      <c r="Z18" s="23" t="s">
-        <v>22</v>
-      </c>
+      <c r="Z18" s="29"/>
       <c r="AA18" s="23" t="s">
         <v>22</v>
       </c>
       <c r="AB18" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC18" s="23" t="s">
         <v>21</v>
-      </c>
-      <c r="AC18" s="29" t="s">
-        <v>65</v>
       </c>
       <c r="AD18" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="AE18" s="29"/>
-      <c r="AF18" s="23" t="s">
+      <c r="AE18" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF18" s="29"/>
+      <c r="AG18" s="23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:33" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="19" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="C19" s="28"/>
       <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
+      <c r="E19" s="28" t="s">
+        <v>65</v>
+      </c>
       <c r="F19" s="28" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="G19" s="19" t="s">
         <v>21</v>
       </c>
       <c r="H19" s="19" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="I19" s="19" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="J19" s="19" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="K19" s="19" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="L19" s="28" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="M19" s="19" t="s">
         <v>21</v>
@@ -8725,60 +8789,63 @@
       </c>
       <c r="V19" s="28"/>
       <c r="W19" s="28"/>
-      <c r="X19" s="28" t="s">
+      <c r="X19" s="28"/>
+      <c r="Y19" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="Y19" s="28"/>
-      <c r="Z19" s="19" t="s">
-        <v>22</v>
-      </c>
+      <c r="Z19" s="28"/>
       <c r="AA19" s="19" t="s">
         <v>22</v>
       </c>
       <c r="AB19" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC19" s="19" t="s">
         <v>21</v>
-      </c>
-      <c r="AC19" s="28" t="s">
-        <v>65</v>
       </c>
       <c r="AD19" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="AE19" s="28"/>
-      <c r="AF19" s="19" t="s">
+      <c r="AE19" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF19" s="28"/>
+      <c r="AG19" s="19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:33" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="23" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="C20" s="29"/>
       <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
+      <c r="E20" s="29" t="s">
+        <v>65</v>
+      </c>
       <c r="F20" s="29" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="G20" s="23" t="s">
         <v>22</v>
       </c>
       <c r="H20" s="23" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="I20" s="23" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="J20" s="23" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="K20" s="23" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="L20" s="29" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="M20" s="23" t="s">
         <v>21</v>
@@ -8809,60 +8876,63 @@
       </c>
       <c r="V20" s="29"/>
       <c r="W20" s="29"/>
-      <c r="X20" s="29" t="s">
+      <c r="X20" s="29"/>
+      <c r="Y20" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="Y20" s="29"/>
-      <c r="Z20" s="23" t="s">
-        <v>22</v>
-      </c>
+      <c r="Z20" s="29"/>
       <c r="AA20" s="23" t="s">
         <v>22</v>
       </c>
       <c r="AB20" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC20" s="23" t="s">
         <v>21</v>
-      </c>
-      <c r="AC20" s="29" t="s">
-        <v>65</v>
       </c>
       <c r="AD20" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="AE20" s="29"/>
-      <c r="AF20" s="23" t="s">
+      <c r="AE20" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF20" s="29"/>
+      <c r="AG20" s="23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:33" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="19" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C21" s="28"/>
       <c r="D21" s="28"/>
-      <c r="E21" s="28"/>
+      <c r="E21" s="28" t="s">
+        <v>65</v>
+      </c>
       <c r="F21" s="28" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="G21" s="19" t="s">
         <v>21</v>
       </c>
       <c r="H21" s="19" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="I21" s="19" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="J21" s="19" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="K21" s="19" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="L21" s="28" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="M21" s="19" t="s">
         <v>21</v>
@@ -8893,60 +8963,63 @@
       </c>
       <c r="V21" s="28"/>
       <c r="W21" s="28"/>
-      <c r="X21" s="28" t="s">
+      <c r="X21" s="28"/>
+      <c r="Y21" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="Y21" s="28"/>
-      <c r="Z21" s="19" t="s">
-        <v>21</v>
-      </c>
+      <c r="Z21" s="28"/>
       <c r="AA21" s="19" t="s">
         <v>21</v>
       </c>
       <c r="AB21" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="AC21" s="28" t="s">
-        <v>65</v>
+      <c r="AC21" s="19" t="s">
+        <v>21</v>
       </c>
       <c r="AD21" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="AE21" s="28"/>
-      <c r="AF21" s="19" t="s">
+      <c r="AE21" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF21" s="28"/>
+      <c r="AG21" s="19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:33" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="23" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="C22" s="29"/>
       <c r="D22" s="29"/>
-      <c r="E22" s="29"/>
+      <c r="E22" s="29" t="s">
+        <v>65</v>
+      </c>
       <c r="F22" s="29" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="G22" s="23" t="s">
         <v>21</v>
       </c>
       <c r="H22" s="23" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="I22" s="23" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="J22" s="23" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="K22" s="23" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="L22" s="29" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="M22" s="23" t="s">
         <v>21</v>
@@ -8977,60 +9050,63 @@
       </c>
       <c r="V22" s="29"/>
       <c r="W22" s="29"/>
-      <c r="X22" s="29" t="s">
+      <c r="X22" s="29"/>
+      <c r="Y22" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="Y22" s="29"/>
-      <c r="Z22" s="23" t="s">
-        <v>21</v>
-      </c>
+      <c r="Z22" s="29"/>
       <c r="AA22" s="23" t="s">
         <v>21</v>
       </c>
       <c r="AB22" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="AC22" s="29" t="s">
-        <v>65</v>
+      <c r="AC22" s="23" t="s">
+        <v>21</v>
       </c>
       <c r="AD22" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="AE22" s="29"/>
-      <c r="AF22" s="23" t="s">
+      <c r="AE22" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF22" s="29"/>
+      <c r="AG22" s="23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:33" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="19" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="C23" s="28"/>
       <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
+      <c r="E23" s="28" t="s">
+        <v>65</v>
+      </c>
       <c r="F23" s="28" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="G23" s="19" t="s">
         <v>22</v>
       </c>
       <c r="H23" s="19" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="I23" s="19" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="J23" s="19" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="K23" s="19" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="L23" s="28" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="M23" s="19" t="s">
         <v>21</v>
@@ -9061,60 +9137,63 @@
       </c>
       <c r="V23" s="28"/>
       <c r="W23" s="28"/>
-      <c r="X23" s="28" t="s">
+      <c r="X23" s="28"/>
+      <c r="Y23" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="Y23" s="28"/>
-      <c r="Z23" s="19" t="s">
-        <v>21</v>
-      </c>
+      <c r="Z23" s="28"/>
       <c r="AA23" s="19" t="s">
         <v>21</v>
       </c>
       <c r="AB23" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="AC23" s="28" t="s">
-        <v>65</v>
+      <c r="AC23" s="19" t="s">
+        <v>21</v>
       </c>
       <c r="AD23" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="AE23" s="28"/>
-      <c r="AF23" s="19" t="s">
+      <c r="AE23" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF23" s="28"/>
+      <c r="AG23" s="19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:33" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="23" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="C24" s="29"/>
       <c r="D24" s="29"/>
-      <c r="E24" s="29"/>
+      <c r="E24" s="29" t="s">
+        <v>65</v>
+      </c>
       <c r="F24" s="29" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="G24" s="23" t="s">
         <v>21</v>
       </c>
       <c r="H24" s="23" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="I24" s="23" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="J24" s="23" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="K24" s="23" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="L24" s="29" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="M24" s="23" t="s">
         <v>21</v>
@@ -9145,60 +9224,63 @@
       </c>
       <c r="V24" s="29"/>
       <c r="W24" s="29"/>
-      <c r="X24" s="29" t="s">
+      <c r="X24" s="29"/>
+      <c r="Y24" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="Y24" s="29"/>
-      <c r="Z24" s="23" t="s">
-        <v>22</v>
-      </c>
+      <c r="Z24" s="29"/>
       <c r="AA24" s="23" t="s">
         <v>22</v>
       </c>
       <c r="AB24" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="AC24" s="29" t="s">
-        <v>65</v>
+      <c r="AC24" s="23" t="s">
+        <v>22</v>
       </c>
       <c r="AD24" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="AE24" s="29"/>
-      <c r="AF24" s="23" t="s">
+      <c r="AE24" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF24" s="29"/>
+      <c r="AG24" s="23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:33" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="19" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="C25" s="28"/>
       <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
+      <c r="E25" s="28" t="s">
+        <v>65</v>
+      </c>
       <c r="F25" s="28" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="G25" s="19" t="s">
         <v>21</v>
       </c>
       <c r="H25" s="19" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="I25" s="19" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="J25" s="19" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="K25" s="19" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="L25" s="28" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="M25" s="19" t="s">
         <v>21</v>
@@ -9229,60 +9311,63 @@
       </c>
       <c r="V25" s="28"/>
       <c r="W25" s="28"/>
-      <c r="X25" s="28" t="s">
+      <c r="X25" s="28"/>
+      <c r="Y25" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="Y25" s="28"/>
-      <c r="Z25" s="19" t="s">
-        <v>22</v>
-      </c>
+      <c r="Z25" s="28"/>
       <c r="AA25" s="19" t="s">
         <v>22</v>
       </c>
       <c r="AB25" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="AC25" s="28" t="s">
-        <v>65</v>
+      <c r="AC25" s="19" t="s">
+        <v>22</v>
       </c>
       <c r="AD25" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="AE25" s="28"/>
-      <c r="AF25" s="19" t="s">
+      <c r="AE25" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF25" s="28"/>
+      <c r="AG25" s="19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:33" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="23" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="C26" s="29"/>
       <c r="D26" s="29"/>
-      <c r="E26" s="29"/>
+      <c r="E26" s="29" t="s">
+        <v>65</v>
+      </c>
       <c r="F26" s="29" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="G26" s="23" t="s">
         <v>22</v>
       </c>
       <c r="H26" s="23" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="I26" s="23" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="J26" s="23" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="K26" s="23" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="L26" s="29" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="M26" s="23" t="s">
         <v>21</v>
@@ -9313,31 +9398,32 @@
       </c>
       <c r="V26" s="29"/>
       <c r="W26" s="29"/>
-      <c r="X26" s="29" t="s">
+      <c r="X26" s="29"/>
+      <c r="Y26" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="Y26" s="29"/>
-      <c r="Z26" s="23" t="s">
-        <v>22</v>
-      </c>
+      <c r="Z26" s="29"/>
       <c r="AA26" s="23" t="s">
         <v>22</v>
       </c>
       <c r="AB26" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="AC26" s="29" t="s">
-        <v>65</v>
+      <c r="AC26" s="23" t="s">
+        <v>22</v>
       </c>
       <c r="AD26" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="AE26" s="29"/>
-      <c r="AF26" s="23" t="s">
+      <c r="AE26" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF26" s="29"/>
+      <c r="AG26" s="23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:33" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="19"/>
       <c r="B27" s="19"/>
       <c r="C27" s="28"/>
@@ -9363,15 +9449,16 @@
       <c r="W27" s="28"/>
       <c r="X27" s="28"/>
       <c r="Y27" s="28"/>
-      <c r="Z27" s="19"/>
+      <c r="Z27" s="28"/>
       <c r="AA27" s="19"/>
       <c r="AB27" s="19"/>
-      <c r="AC27" s="28"/>
+      <c r="AC27" s="19"/>
       <c r="AD27" s="28"/>
       <c r="AE27" s="28"/>
-      <c r="AF27" s="19"/>
-    </row>
-    <row r="28" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AF27" s="28"/>
+      <c r="AG27" s="19"/>
+    </row>
+    <row r="28" spans="1:33" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="23"/>
       <c r="B28" s="23"/>
       <c r="C28" s="29"/>
@@ -9397,17 +9484,18 @@
       <c r="W28" s="29"/>
       <c r="X28" s="29"/>
       <c r="Y28" s="29"/>
-      <c r="Z28" s="23"/>
+      <c r="Z28" s="29"/>
       <c r="AA28" s="23"/>
       <c r="AB28" s="23"/>
-      <c r="AC28" s="29"/>
+      <c r="AC28" s="23"/>
       <c r="AD28" s="29"/>
       <c r="AE28" s="29"/>
-      <c r="AF28" s="23"/>
-    </row>
-    <row r="30" spans="1:32" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AF28" s="29"/>
+      <c r="AG28" s="23"/>
+    </row>
+    <row r="30" spans="1:33" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="78" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="B30" s="78"/>
       <c r="C30" s="78"/>
@@ -9429,10 +9517,10 @@
       <c r="S30" s="62"/>
       <c r="T30" s="62"/>
     </row>
-    <row r="31" spans="1:32" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:33" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="11"/>
       <c r="B31" s="80" t="s">
-        <v>758</v>
+        <v>769</v>
       </c>
       <c r="C31" s="80"/>
       <c r="D31" s="80"/>
@@ -9453,34 +9541,34 @@
       <c r="S31" s="80"/>
       <c r="T31" s="80"/>
     </row>
-    <row r="32" spans="1:32" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:33" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="8"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="D32" s="8" t="s">
         <v>502</v>
       </c>
-      <c r="E32" s="83" t="s">
-        <v>673</v>
-      </c>
-      <c r="F32" s="84"/>
-      <c r="G32" s="85"/>
+      <c r="E32" s="82" t="s">
+        <v>671</v>
+      </c>
+      <c r="F32" s="83"/>
+      <c r="G32" s="84"/>
       <c r="H32" s="8" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
       <c r="J32" s="8" t="s">
+        <v>750</v>
+      </c>
+      <c r="K32" s="8" t="s">
         <v>753</v>
       </c>
-      <c r="K32" s="8" t="s">
-        <v>756</v>
-      </c>
       <c r="L32" s="8" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="M32" s="8"/>
       <c r="N32" s="8"/>
@@ -9496,37 +9584,37 @@
         <v>0</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>765</v>
+        <v>760</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>754</v>
+        <v>751</v>
       </c>
       <c r="H33" s="8" t="s">
+        <v>672</v>
+      </c>
+      <c r="I33" s="8" t="s">
+        <v>673</v>
+      </c>
+      <c r="J33" s="8" t="s">
         <v>674</v>
       </c>
-      <c r="I33" s="8" t="s">
+      <c r="K33" s="8" t="s">
+        <v>650</v>
+      </c>
+      <c r="L33" s="8" t="s">
         <v>675</v>
-      </c>
-      <c r="J33" s="8" t="s">
-        <v>676</v>
-      </c>
-      <c r="K33" s="8" t="s">
-        <v>652</v>
-      </c>
-      <c r="L33" s="8" t="s">
-        <v>677</v>
       </c>
       <c r="M33" s="8"/>
       <c r="N33" s="8"/>
@@ -9539,7 +9627,7 @@
     </row>
     <row r="34" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="19" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="B34" s="19" t="s">
         <v>512</v>
@@ -9561,7 +9649,7 @@
         <v>21</v>
       </c>
       <c r="I34" s="19" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
       <c r="J34" s="19" t="s">
         <v>21</v>
@@ -9579,7 +9667,7 @@
     </row>
     <row r="35" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="23" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="B35" s="23" t="s">
         <v>513</v>
@@ -9601,7 +9689,7 @@
         <v>21</v>
       </c>
       <c r="I35" s="23" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
       <c r="J35" s="23" t="s">
         <v>21</v>
@@ -9751,7 +9839,7 @@
     </row>
     <row r="43" spans="1:20" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="78" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="B43" s="78"/>
       <c r="C43" s="78"/>
@@ -9776,7 +9864,7 @@
     <row r="44" spans="1:20" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="11"/>
       <c r="B44" s="80" t="s">
-        <v>758</v>
+        <v>769</v>
       </c>
       <c r="C44" s="80"/>
       <c r="D44" s="80"/>
@@ -9801,13 +9889,13 @@
       <c r="A45" s="8"/>
       <c r="B45" s="8"/>
       <c r="C45" s="8" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="D45" s="8" t="s">
         <v>502</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="F45" s="8" t="s">
         <v>506</v>
@@ -9832,19 +9920,19 @@
         <v>0</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="G46" s="8"/>
       <c r="H46" s="8"/>
@@ -9863,7 +9951,7 @@
     </row>
     <row r="47" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="19" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B47" s="19" t="s">
         <v>65</v>
@@ -9871,7 +9959,7 @@
       <c r="C47" s="28"/>
       <c r="D47" s="28"/>
       <c r="E47" s="19" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="F47" s="28" t="s">
         <v>65</v>
@@ -9915,7 +10003,7 @@
     </row>
     <row r="50" spans="1:32" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="78" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="B50" s="78"/>
       <c r="C50" s="78"/>
@@ -9952,7 +10040,7 @@
     <row r="51" spans="1:32" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="11"/>
       <c r="B51" s="80" t="s">
-        <v>758</v>
+        <v>769</v>
       </c>
       <c r="C51" s="80"/>
       <c r="D51" s="80"/>
@@ -9989,88 +10077,88 @@
       <c r="A52" s="8"/>
       <c r="B52" s="8"/>
       <c r="C52" s="8" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="D52" s="8" t="s">
         <v>502</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="G52" s="8" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="H52" s="8" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="I52" s="8" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="J52" s="8" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="K52" s="8" t="s">
-        <v>745</v>
+        <v>768</v>
       </c>
       <c r="L52" s="8" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="M52" s="8" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="N52" s="8" t="s">
         <v>505</v>
       </c>
       <c r="O52" s="8" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="P52" s="8" t="s">
+        <v>722</v>
+      </c>
+      <c r="Q52" s="8" t="s">
+        <v>723</v>
+      </c>
+      <c r="R52" s="8" t="s">
         <v>724</v>
       </c>
-      <c r="Q52" s="8" t="s">
+      <c r="S52" s="8" t="s">
+        <v>740</v>
+      </c>
+      <c r="T52" s="8" t="s">
+        <v>743</v>
+      </c>
+      <c r="U52" s="8" t="s">
         <v>725</v>
       </c>
-      <c r="R52" s="8" t="s">
+      <c r="V52" s="8" t="s">
+        <v>691</v>
+      </c>
+      <c r="W52" s="8" t="s">
         <v>726</v>
-      </c>
-      <c r="S52" s="8" t="s">
-        <v>742</v>
-      </c>
-      <c r="T52" s="8" t="s">
-        <v>746</v>
-      </c>
-      <c r="U52" s="8" t="s">
-        <v>727</v>
-      </c>
-      <c r="V52" s="8" t="s">
-        <v>693</v>
-      </c>
-      <c r="W52" s="8" t="s">
-        <v>728</v>
       </c>
       <c r="X52" s="8" t="s">
         <v>506</v>
       </c>
       <c r="Y52" s="8" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="Z52" s="8" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="AA52" s="63" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="AB52" s="64" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="AC52" s="64" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
       <c r="AD52" s="64" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="AE52" s="8"/>
       <c r="AF52" s="8"/>
@@ -10080,106 +10168,106 @@
         <v>0</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>558</v>
+        <v>766</v>
       </c>
       <c r="F53" s="8" t="s">
-        <v>559</v>
+        <v>767</v>
       </c>
       <c r="G53" s="8" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="H53" s="8" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="I53" s="8" t="s">
+        <v>732</v>
+      </c>
+      <c r="J53" s="8" t="s">
+        <v>735</v>
+      </c>
+      <c r="K53" s="8" t="s">
+        <v>737</v>
+      </c>
+      <c r="L53" s="8" t="s">
+        <v>738</v>
+      </c>
+      <c r="M53" s="8" t="s">
+        <v>677</v>
+      </c>
+      <c r="N53" s="8" t="s">
+        <v>680</v>
+      </c>
+      <c r="O53" s="8" t="s">
+        <v>676</v>
+      </c>
+      <c r="P53" s="8" t="s">
+        <v>729</v>
+      </c>
+      <c r="Q53" s="8" t="s">
+        <v>730</v>
+      </c>
+      <c r="R53" s="8" t="s">
+        <v>617</v>
+      </c>
+      <c r="S53" s="8" t="s">
+        <v>739</v>
+      </c>
+      <c r="T53" s="8" t="s">
+        <v>678</v>
+      </c>
+      <c r="U53" s="8" t="s">
+        <v>683</v>
+      </c>
+      <c r="V53" s="8" t="s">
+        <v>669</v>
+      </c>
+      <c r="W53" s="8" t="s">
+        <v>681</v>
+      </c>
+      <c r="X53" s="8" t="s">
+        <v>625</v>
+      </c>
+      <c r="Y53" s="8" t="s">
+        <v>731</v>
+      </c>
+      <c r="Z53" s="8" t="s">
+        <v>686</v>
+      </c>
+      <c r="AA53" s="8" t="s">
+        <v>679</v>
+      </c>
+      <c r="AB53" s="8" t="s">
+        <v>736</v>
+      </c>
+      <c r="AC53" s="8" t="s">
+        <v>733</v>
+      </c>
+      <c r="AD53" s="8" t="s">
         <v>734</v>
-      </c>
-      <c r="J53" s="8" t="s">
-        <v>737</v>
-      </c>
-      <c r="K53" s="8" t="s">
-        <v>739</v>
-      </c>
-      <c r="L53" s="8" t="s">
-        <v>740</v>
-      </c>
-      <c r="M53" s="8" t="s">
-        <v>679</v>
-      </c>
-      <c r="N53" s="8" t="s">
-        <v>682</v>
-      </c>
-      <c r="O53" s="8" t="s">
-        <v>678</v>
-      </c>
-      <c r="P53" s="8" t="s">
-        <v>731</v>
-      </c>
-      <c r="Q53" s="8" t="s">
-        <v>732</v>
-      </c>
-      <c r="R53" s="8" t="s">
-        <v>619</v>
-      </c>
-      <c r="S53" s="8" t="s">
-        <v>741</v>
-      </c>
-      <c r="T53" s="8" t="s">
-        <v>680</v>
-      </c>
-      <c r="U53" s="8" t="s">
-        <v>685</v>
-      </c>
-      <c r="V53" s="8" t="s">
-        <v>671</v>
-      </c>
-      <c r="W53" s="8" t="s">
-        <v>683</v>
-      </c>
-      <c r="X53" s="8" t="s">
-        <v>627</v>
-      </c>
-      <c r="Y53" s="8" t="s">
-        <v>733</v>
-      </c>
-      <c r="Z53" s="8" t="s">
-        <v>688</v>
-      </c>
-      <c r="AA53" s="8" t="s">
-        <v>681</v>
-      </c>
-      <c r="AB53" s="8" t="s">
-        <v>738</v>
-      </c>
-      <c r="AC53" s="8" t="s">
-        <v>735</v>
-      </c>
-      <c r="AD53" s="8" t="s">
-        <v>736</v>
       </c>
       <c r="AE53" s="8"/>
       <c r="AF53" s="8"/>
     </row>
     <row r="54" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="19" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="B54" s="19" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="C54" s="28"/>
       <c r="D54" s="28"/>
       <c r="E54" s="28" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="F54" s="27"/>
       <c r="G54" s="27"/>
@@ -10193,22 +10281,22 @@
         <v>21</v>
       </c>
       <c r="O54" s="19" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="P54" s="28"/>
       <c r="Q54" s="28"/>
       <c r="R54" s="19" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="S54" s="28"/>
       <c r="T54" s="19" t="s">
         <v>48</v>
       </c>
       <c r="U54" s="19" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="V54" s="19" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="W54" s="19" t="s">
         <v>507</v>
@@ -10231,15 +10319,15 @@
     </row>
     <row r="55" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="23" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="B55" s="23" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="C55" s="29"/>
       <c r="D55" s="29"/>
       <c r="E55" s="29" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="F55" s="24"/>
       <c r="G55" s="24"/>
@@ -10253,22 +10341,22 @@
         <v>21</v>
       </c>
       <c r="O55" s="23" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="P55" s="29"/>
       <c r="Q55" s="29"/>
       <c r="R55" s="29" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="S55" s="29"/>
       <c r="T55" s="23" t="s">
         <v>48</v>
       </c>
       <c r="U55" s="23" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="V55" s="29" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="W55" s="29" t="s">
         <v>507</v>
@@ -10631,11 +10719,13 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="U12:Y12"/>
-    <mergeCell ref="Z12:AB12"/>
-    <mergeCell ref="AC12:AF12"/>
     <mergeCell ref="B44:T44"/>
     <mergeCell ref="E32:G32"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:T12"/>
+    <mergeCell ref="U12:Z12"/>
+    <mergeCell ref="AA12:AC12"/>
+    <mergeCell ref="AD12:AG12"/>
     <mergeCell ref="B51:T51"/>
     <mergeCell ref="B31:T31"/>
     <mergeCell ref="A1:Q1"/>
@@ -10643,13 +10733,11 @@
     <mergeCell ref="A30:Q30"/>
     <mergeCell ref="A43:Q43"/>
     <mergeCell ref="A50:Q50"/>
-    <mergeCell ref="D12:T12"/>
-    <mergeCell ref="A12:C12"/>
     <mergeCell ref="B2:T2"/>
     <mergeCell ref="B11:T11"/>
   </mergeCells>
   <dataValidations count="25">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Extend Outside ACI" error="Valid answers are no or yes" sqref="E34:H41 N54:N65 J34:J41 C34:C41 Z15:AB28 G15:G28 AF15:AF28 P15:Q28 M15:N28 U15:U28 Z54:AA65" xr:uid="{E7480C92-0A40-41D3-A6A4-8664870402A9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Extend Outside ACI" error="Valid answers are no or yes" sqref="E34:H41 N54:N65 J34:J41 C34:C41 AA15:AC28 G15:G28 AG15:AG28 P15:Q28 M15:N28 U15:U28 Z54:AA65" xr:uid="{E7480C92-0A40-41D3-A6A4-8664870402A9}">
       <formula1>"no,yes"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="VPC ID" error="The VPC ID must be a number between 1 and 1000" sqref="B54:B65 B5:B8 B47:B48 B34:B41 D34:D41 B15:B28" xr:uid="{473BF0FF-FE43-43B6-BA03-96E475D106E1}"/>
@@ -11487,7 +11575,7 @@
     <row r="2" spans="1:13" ht="51" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13"/>
       <c r="B2" s="67" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="C2" s="67"/>
       <c r="D2" s="67"/>
@@ -11675,7 +11763,7 @@
     <row r="11" spans="1:13" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="11"/>
       <c r="B11" s="72" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="C11" s="72"/>
       <c r="D11" s="72"/>
@@ -12651,7 +12739,7 @@
     <row r="18" spans="1:30" s="6" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="11"/>
       <c r="B18" s="65" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="C18" s="65"/>
       <c r="D18" s="65"/>
@@ -13895,7 +13983,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="69" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B1" s="69"/>
       <c r="C1" s="69"/>
@@ -13914,7 +14002,7 @@
     <row r="2" spans="1:14" ht="87.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="10"/>
       <c r="B2" s="73" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C2" s="73"/>
       <c r="D2" s="73"/>
@@ -14034,7 +14122,7 @@
     <row r="8" spans="1:14" ht="63.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="15"/>
       <c r="B8" s="76" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="C8" s="76"/>
       <c r="D8" s="76"/>
@@ -14174,7 +14262,7 @@
     <row r="14" spans="1:14" ht="69.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15"/>
       <c r="B14" s="76" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="C14" s="76"/>
       <c r="D14" s="76"/>
@@ -14313,7 +14401,7 @@
     <row r="20" spans="1:13" customFormat="1" ht="51.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="55"/>
       <c r="B20" s="74" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="C20" s="75"/>
       <c r="D20" s="75"/>
@@ -14414,7 +14502,7 @@
     <row r="26" spans="1:13" ht="203.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="13"/>
       <c r="B26" s="67" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="C26" s="67"/>
       <c r="D26" s="67"/>
@@ -14726,7 +14814,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>511</v>
@@ -15154,7 +15242,7 @@
     <row r="2" spans="1:13" s="6" customFormat="1" ht="184.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="79" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="C2" s="79"/>
       <c r="D2" s="79"/>
@@ -15173,7 +15261,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>511</v>
@@ -15188,7 +15276,7 @@
         <v>30</v>
       </c>
       <c r="G3" s="54" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="H3" s="54"/>
       <c r="I3" s="54"/>
@@ -15202,7 +15290,7 @@
         <v>162</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C4" s="19"/>
       <c r="D4" s="28" t="s">
@@ -15215,7 +15303,7 @@
         <v>459</v>
       </c>
       <c r="G4" s="28" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="H4" s="28"/>
       <c r="I4" s="28"/>
@@ -15229,7 +15317,7 @@
         <v>162</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="29" t="s">
@@ -15242,7 +15330,7 @@
         <v>467</v>
       </c>
       <c r="G5" s="29" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="H5" s="29"/>
       <c r="I5" s="29"/>
@@ -15421,7 +15509,7 @@
     <row r="18" spans="1:13" s="6" customFormat="1" ht="241.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="11"/>
       <c r="B18" s="65" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="C18" s="65"/>
       <c r="D18" s="65"/>
@@ -15732,7 +15820,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="78" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="B1" s="78"/>
       <c r="C1" s="78"/>
@@ -16174,7 +16262,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="78" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="B1" s="78"/>
       <c r="C1" s="78"/>
@@ -16198,7 +16286,7 @@
     <row r="2" spans="1:19" ht="390" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="79" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="C2" s="79"/>
       <c r="D2" s="79"/>
@@ -16223,7 +16311,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>511</v>
@@ -16244,10 +16332,10 @@
         <v>161</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="K3" s="8" t="s">
         <v>499</v>
@@ -16282,7 +16370,7 @@
         <v>504</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C4" s="19"/>
       <c r="D4" s="19" t="s">
@@ -16317,7 +16405,7 @@
         <v>169</v>
       </c>
       <c r="Q4" s="28" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="R4" s="27">
         <v>56</v>
@@ -16329,7 +16417,7 @@
         <v>504</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="23" t="s">
@@ -16364,7 +16452,7 @@
         <v>171</v>
       </c>
       <c r="Q5" s="29" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="R5" s="24">
         <v>995</v>
@@ -16376,7 +16464,7 @@
         <v>504</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C6" s="19"/>
       <c r="D6" s="19" t="s">
@@ -16411,7 +16499,7 @@
         <v>172</v>
       </c>
       <c r="Q6" s="28" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="R6" s="27">
         <v>996</v>
@@ -16423,7 +16511,7 @@
         <v>504</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C7" s="23"/>
       <c r="D7" s="23" t="s">
@@ -16458,7 +16546,7 @@
         <v>173</v>
       </c>
       <c r="Q7" s="29" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="R7" s="24">
         <v>999</v>
@@ -16470,7 +16558,7 @@
         <v>504</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C8" s="19"/>
       <c r="D8" s="19" t="s">
@@ -16503,7 +16591,7 @@
       </c>
       <c r="P8" s="41"/>
       <c r="Q8" s="28" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="R8" s="27">
         <v>1</v>
@@ -16515,7 +16603,7 @@
         <v>504</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C9" s="23"/>
       <c r="D9" s="23" t="s">
@@ -16550,7 +16638,7 @@
         <v>174</v>
       </c>
       <c r="Q9" s="29" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="R9" s="24">
         <v>64</v>
@@ -16562,7 +16650,7 @@
         <v>504</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C10" s="19"/>
       <c r="D10" s="19" t="s">
@@ -16597,7 +16685,7 @@
         <v>175</v>
       </c>
       <c r="Q10" s="28" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="R10" s="27">
         <v>80</v>
@@ -16609,7 +16697,7 @@
         <v>504</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C11" s="23"/>
       <c r="D11" s="23" t="s">
@@ -16642,7 +16730,7 @@
       </c>
       <c r="P11" s="58"/>
       <c r="Q11" s="29" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="R11" s="24">
         <v>87</v>
@@ -16654,7 +16742,7 @@
         <v>504</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C12" s="19"/>
       <c r="D12" s="19" t="s">
@@ -16689,7 +16777,7 @@
         <v>176</v>
       </c>
       <c r="Q12" s="28" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="R12" s="27">
         <v>90</v>
@@ -16701,7 +16789,7 @@
         <v>504</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C13" s="23"/>
       <c r="D13" s="23" t="s">
@@ -16736,7 +16824,7 @@
         <v>177</v>
       </c>
       <c r="Q13" s="29" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="R13" s="24">
         <v>91</v>
@@ -16748,7 +16836,7 @@
         <v>504</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C14" s="19"/>
       <c r="D14" s="19" t="s">
@@ -16783,7 +16871,7 @@
         <v>178</v>
       </c>
       <c r="Q14" s="28" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="R14" s="27">
         <v>110</v>
@@ -16795,7 +16883,7 @@
         <v>504</v>
       </c>
       <c r="B15" s="29" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C15" s="23"/>
       <c r="D15" s="23" t="s">
@@ -16828,7 +16916,7 @@
       </c>
       <c r="P15" s="58"/>
       <c r="Q15" s="29" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="R15" s="24">
         <v>136</v>
@@ -16840,7 +16928,7 @@
         <v>504</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C16" s="19"/>
       <c r="D16" s="19" t="s">
@@ -16875,7 +16963,7 @@
         <v>179</v>
       </c>
       <c r="Q16" s="28" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="R16" s="27">
         <v>168</v>
@@ -16887,7 +16975,7 @@
         <v>504</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C17" s="23"/>
       <c r="D17" s="23" t="s">
@@ -16922,7 +17010,7 @@
         <v>180</v>
       </c>
       <c r="Q17" s="29" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="R17" s="24">
         <v>169</v>
@@ -16934,7 +17022,7 @@
         <v>504</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C18" s="19"/>
       <c r="D18" s="19" t="s">
@@ -16969,7 +17057,7 @@
         <v>181</v>
       </c>
       <c r="Q18" s="28" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="R18" s="27">
         <v>691</v>
@@ -16981,7 +17069,7 @@
         <v>504</v>
       </c>
       <c r="B19" s="29" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C19" s="23"/>
       <c r="D19" s="23" t="s">
@@ -17016,7 +17104,7 @@
         <v>182</v>
       </c>
       <c r="Q19" s="29" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="R19" s="24">
         <v>811</v>
@@ -17028,7 +17116,7 @@
         <v>504</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C20" s="19"/>
       <c r="D20" s="19" t="s">
@@ -17063,7 +17151,7 @@
         <v>183</v>
       </c>
       <c r="Q20" s="28" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="R20" s="27">
         <v>812</v>
@@ -17075,7 +17163,7 @@
         <v>504</v>
       </c>
       <c r="B21" s="29" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C21" s="23"/>
       <c r="D21" s="23" t="s">
@@ -17110,7 +17198,7 @@
         <v>184</v>
       </c>
       <c r="Q21" s="29" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="R21" s="24">
         <v>997</v>
@@ -17122,7 +17210,7 @@
         <v>504</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C22" s="19"/>
       <c r="D22" s="19" t="s">
@@ -17157,7 +17245,7 @@
         <v>184</v>
       </c>
       <c r="Q22" s="28" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="R22" s="27">
         <v>998</v>
@@ -17169,7 +17257,7 @@
         <v>504</v>
       </c>
       <c r="B23" s="29" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C23" s="23"/>
       <c r="D23" s="23" t="s">
@@ -17204,7 +17292,7 @@
         <v>185</v>
       </c>
       <c r="Q23" s="29" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="R23" s="24">
         <v>3001</v>
@@ -17216,7 +17304,7 @@
         <v>504</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C24" s="19"/>
       <c r="D24" s="19" t="s">
@@ -17249,7 +17337,7 @@
       </c>
       <c r="P24" s="41"/>
       <c r="Q24" s="28" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="R24" s="27">
         <v>3003</v>
@@ -17261,7 +17349,7 @@
         <v>504</v>
       </c>
       <c r="B25" s="29" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C25" s="23"/>
       <c r="D25" s="23" t="s">
@@ -17296,7 +17384,7 @@
         <v>186</v>
       </c>
       <c r="Q25" s="29" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="R25" s="24">
         <v>3004</v>
@@ -17308,7 +17396,7 @@
         <v>504</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C26" s="19"/>
       <c r="D26" s="19" t="s">
@@ -17341,7 +17429,7 @@
       </c>
       <c r="P26" s="41"/>
       <c r="Q26" s="28" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="R26" s="27">
         <v>3006</v>
@@ -17353,7 +17441,7 @@
         <v>504</v>
       </c>
       <c r="B27" s="29" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C27" s="23"/>
       <c r="D27" s="23" t="s">
@@ -17386,7 +17474,7 @@
       </c>
       <c r="P27" s="58"/>
       <c r="Q27" s="29" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="R27" s="24">
         <v>3007</v>
@@ -17398,7 +17486,7 @@
         <v>504</v>
       </c>
       <c r="B28" s="28" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C28" s="19"/>
       <c r="D28" s="19" t="s">
@@ -17431,7 +17519,7 @@
       </c>
       <c r="P28" s="41"/>
       <c r="Q28" s="28" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="R28" s="27">
         <v>3011</v>
@@ -17443,7 +17531,7 @@
         <v>504</v>
       </c>
       <c r="B29" s="29" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C29" s="23"/>
       <c r="D29" s="23" t="s">
@@ -17476,7 +17564,7 @@
       </c>
       <c r="P29" s="58"/>
       <c r="Q29" s="29" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="R29" s="24">
         <v>3019</v>
@@ -17488,7 +17576,7 @@
         <v>504</v>
       </c>
       <c r="B30" s="28" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C30" s="19"/>
       <c r="D30" s="19" t="s">
@@ -17523,7 +17611,7 @@
         <v>187</v>
       </c>
       <c r="Q30" s="28" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="R30" s="27">
         <v>3103</v>
@@ -17535,7 +17623,7 @@
         <v>504</v>
       </c>
       <c r="B31" s="29" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C31" s="23"/>
       <c r="D31" s="23" t="s">
@@ -17570,7 +17658,7 @@
         <v>188</v>
       </c>
       <c r="Q31" s="29" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="R31" s="24">
         <v>3910</v>
@@ -17582,7 +17670,7 @@
         <v>504</v>
       </c>
       <c r="B32" s="28" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C32" s="19"/>
       <c r="D32" s="19" t="s">
@@ -17617,7 +17705,7 @@
         <v>189</v>
       </c>
       <c r="Q32" s="28" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="R32" s="27">
         <v>3960</v>
@@ -17629,7 +17717,7 @@
         <v>504</v>
       </c>
       <c r="B33" s="29" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C33" s="23"/>
       <c r="D33" s="23" t="s">
@@ -17664,7 +17752,7 @@
         <v>190</v>
       </c>
       <c r="Q33" s="29" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="R33" s="24">
         <v>3961</v>
@@ -17676,7 +17764,7 @@
         <v>504</v>
       </c>
       <c r="B34" s="28" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C34" s="19"/>
       <c r="D34" s="19" t="s">
@@ -17711,7 +17799,7 @@
         <v>191</v>
       </c>
       <c r="Q34" s="28" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="R34" s="27">
         <v>3962</v>
@@ -17723,7 +17811,7 @@
         <v>504</v>
       </c>
       <c r="B35" s="29" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C35" s="23"/>
       <c r="D35" s="23" t="s">
@@ -17758,7 +17846,7 @@
         <v>192</v>
       </c>
       <c r="Q35" s="29" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="R35" s="24">
         <v>3963</v>
@@ -17770,7 +17858,7 @@
         <v>504</v>
       </c>
       <c r="B36" s="28" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C36" s="19"/>
       <c r="D36" s="19" t="s">
@@ -17805,7 +17893,7 @@
         <v>193</v>
       </c>
       <c r="Q36" s="28" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="R36" s="27">
         <v>3964</v>
@@ -17817,7 +17905,7 @@
         <v>504</v>
       </c>
       <c r="B37" s="29" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C37" s="23"/>
       <c r="D37" s="23" t="s">
@@ -17852,7 +17940,7 @@
         <v>194</v>
       </c>
       <c r="Q37" s="29" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="R37" s="24">
         <v>3965</v>
@@ -17864,7 +17952,7 @@
         <v>504</v>
       </c>
       <c r="B38" s="28" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C38" s="19"/>
       <c r="D38" s="19" t="s">
@@ -17899,7 +17987,7 @@
         <v>195</v>
       </c>
       <c r="Q38" s="28" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="R38" s="27">
         <v>3966</v>
@@ -17911,7 +17999,7 @@
         <v>504</v>
       </c>
       <c r="B39" s="29" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C39" s="23"/>
       <c r="D39" s="23" t="s">
@@ -17946,7 +18034,7 @@
         <v>196</v>
       </c>
       <c r="Q39" s="29" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="R39" s="24">
         <v>3967</v>
@@ -17958,7 +18046,7 @@
         <v>504</v>
       </c>
       <c r="B40" s="28" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C40" s="19"/>
       <c r="D40" s="19" t="s">
@@ -17993,7 +18081,7 @@
         <v>198</v>
       </c>
       <c r="Q40" s="28" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="R40" s="27">
         <v>201</v>
@@ -18005,7 +18093,7 @@
         <v>504</v>
       </c>
       <c r="B41" s="29" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C41" s="23"/>
       <c r="D41" s="23" t="s">
@@ -18040,7 +18128,7 @@
         <v>200</v>
       </c>
       <c r="Q41" s="29" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="R41" s="24">
         <v>202</v>
@@ -18052,7 +18140,7 @@
         <v>504</v>
       </c>
       <c r="B42" s="28" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C42" s="19"/>
       <c r="D42" s="19" t="s">
@@ -18087,7 +18175,7 @@
         <v>202</v>
       </c>
       <c r="Q42" s="28" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="R42" s="27">
         <v>203</v>
@@ -18099,7 +18187,7 @@
         <v>504</v>
       </c>
       <c r="B43" s="29" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C43" s="23"/>
       <c r="D43" s="23" t="s">
@@ -18132,7 +18220,7 @@
         <v>203</v>
       </c>
       <c r="Q43" s="29" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="R43" s="24">
         <v>204</v>
@@ -18144,7 +18232,7 @@
         <v>504</v>
       </c>
       <c r="B44" s="28" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C44" s="19"/>
       <c r="D44" s="19" t="s">
@@ -18177,7 +18265,7 @@
         <v>204</v>
       </c>
       <c r="Q44" s="28" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="R44" s="27">
         <v>205</v>
@@ -18189,7 +18277,7 @@
         <v>504</v>
       </c>
       <c r="B45" s="29" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C45" s="23"/>
       <c r="D45" s="23" t="s">
@@ -18222,7 +18310,7 @@
         <v>205</v>
       </c>
       <c r="Q45" s="29" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="R45" s="24">
         <v>206</v>
@@ -18234,7 +18322,7 @@
         <v>504</v>
       </c>
       <c r="B46" s="28" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C46" s="19"/>
       <c r="D46" s="19" t="s">
@@ -18267,7 +18355,7 @@
         <v>206</v>
       </c>
       <c r="Q46" s="28" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="R46" s="27">
         <v>207</v>

</xml_diff>